<commit_message>
Updated ITA_grids model - 2025-08-21 15:47
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA_grids/Sets-vervestacks.xlsx
+++ b/VerveStacks_ITA_grids/Sets-vervestacks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA_grids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C9288C6-500B-4235-8267-0DCE922460F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB02F128-229A-4C9F-A424-CB8165706819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4942,7 +4942,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F966D63-D68B-FB48-AAA9-71788BE6A8AF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F495A2CE-36F9-7ECF-D868-C2F3234EA13C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5724,7 +5724,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81DAAC70-2D79-407C-B4FF-6C8C30C6D313}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52A40599-F48A-4633-ACF7-880025CC168A}">
   <dimension ref="A1:H737"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA_grids model - 2025-08-23 15:24
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA_grids/Sets-vervestacks.xlsx
+++ b/VerveStacks_ITA_grids/Sets-vervestacks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA_grids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB02F128-229A-4C9F-A424-CB8165706819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{778143B5-FCD6-42BF-B791-4D431EE7E9C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4942,7 +4942,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F495A2CE-36F9-7ECF-D868-C2F3234EA13C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88949F21-B751-1E02-9066-18CE3E0EE15A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5724,7 +5724,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52A40599-F48A-4633-ACF7-880025CC168A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E0A17E9-2EE6-455A-8C8A-D3D1B3686A23}">
   <dimension ref="A1:H737"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA_grids model - 2025-08-29 14:00
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA_grids/Sets-vervestacks.xlsx
+++ b/VerveStacks_ITA_grids/Sets-vervestacks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA_grids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{738047D5-A538-4502-854E-7F66EC0DF8CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C5E68215-3C06-4D95-BA34-F638ED81C264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4942,7 +4942,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8630C52-E05B-93D1-87AC-552863B30200}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04FB1F6C-6FFB-EFDD-EA82-A63A1CA22B0B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5724,7 +5724,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0969A3DF-1686-4E6E-897A-5199BD23A697}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{953B99C9-AA5B-4656-A47A-492BD1351454}">
   <dimension ref="A1:H737"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>